<commit_message>
hw update FDS2-7 and MP1-6
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmac\Google Drive\courses\lossd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D39E98-08A3-4E24-9F73-1CF97FE957F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8026457-2446-4E1A-8D25-8D55F448BE7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -207,24 +207,6 @@
     </r>
   </si>
   <si>
-    <t>FDS 02, due 1/31</t>
-  </si>
-  <si>
-    <t>FDS 03, due 2/7</t>
-  </si>
-  <si>
-    <t>FDS 04, due 2/14</t>
-  </si>
-  <si>
-    <t>FDS 05, due 2/21</t>
-  </si>
-  <si>
-    <t>FDS 06, due 2/28</t>
-  </si>
-  <si>
-    <t>FDS 07, due 3/7</t>
-  </si>
-  <si>
     <t>[college farm visit]</t>
   </si>
   <si>
@@ -238,6 +220,24 @@
   </si>
   <si>
     <t>PR3</t>
+  </si>
+  <si>
+    <t>FDS2, due 1/31</t>
+  </si>
+  <si>
+    <t>FDS3, due 2/7</t>
+  </si>
+  <si>
+    <t>FDS4, due 2/14</t>
+  </si>
+  <si>
+    <t>FDS5, due 2/21</t>
+  </si>
+  <si>
+    <t>FDS6, due 2/28</t>
+  </si>
+  <si>
+    <t>FDS7, due 3/7</t>
   </si>
 </sst>
 </file>
@@ -665,8 +665,8 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,7 +725,7 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="21" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -740,14 +740,14 @@
         <v>44594</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="21" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="21" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -793,7 +793,7 @@
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="21" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -818,7 +818,7 @@
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="21" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -839,7 +839,7 @@
       <c r="F7" s="14"/>
       <c r="G7" s="13"/>
       <c r="H7" s="21" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -927,14 +927,14 @@
         <v>44650</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H12" s="3"/>
     </row>
@@ -976,7 +976,7 @@
       <c r="E14" s="23"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H14" s="3"/>
     </row>
@@ -1016,7 +1016,7 @@
       <c r="E16" s="23"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H16" s="3"/>
     </row>

</xml_diff>

<commit_message>
rename PR1 etc to EPR1
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmac\Google Drive\courses\lossd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E660FBF6-CC95-4062-8550-061242504E1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2818D14-2AC1-4287-A381-AB0608C6743D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,15 +194,6 @@
   </si>
   <si>
     <t>[Matt Steiman visit]</t>
-  </si>
-  <si>
-    <t>PR1</t>
-  </si>
-  <si>
-    <t>PR2</t>
-  </si>
-  <si>
-    <t>PR3</t>
   </si>
   <si>
     <t>FDS2, due 1/31</t>
@@ -257,6 +248,15 @@
       </rPr>
       <t>(due by the start of class)</t>
     </r>
+  </si>
+  <si>
+    <t>EPR1</t>
+  </si>
+  <si>
+    <t>EPR2</t>
+  </si>
+  <si>
+    <t>EPR3</t>
   </si>
 </sst>
 </file>
@@ -693,7 +693,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +727,7 @@
         <v>20</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>37</v>
@@ -752,7 +752,7 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -774,7 +774,7 @@
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -799,7 +799,7 @@
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -820,7 +820,7 @@
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -845,7 +845,7 @@
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -866,7 +866,7 @@
       <c r="F7" s="14"/>
       <c r="G7" s="13"/>
       <c r="H7" s="21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="13" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="H12" s="3"/>
     </row>
@@ -1003,7 +1003,7 @@
       <c r="E14" s="23"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H14" s="3"/>
     </row>
@@ -1043,7 +1043,7 @@
       <c r="E16" s="23"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="H16" s="3"/>
     </row>

</xml_diff>